<commit_message>
making image upload automatic
</commit_message>
<xml_diff>
--- a/Fb.xlsx
+++ b/Fb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A73"/>
+  <dimension ref="A1:A69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,327 +443,292 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Amén</t>
+          <t>Amen amen amen</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Amen amen amen</t>
+          <t>I don't know who you are or what your name is but if you're Reading this, I send healing to your entire body in the name of Jesus</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Breaking News God is going to Double your Blessings this week, get ready to Receive them.</t>
+          <t xml:space="preserve">Amén </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>INFINITAS GRACIAS SEÑOR JESÚS por un día más de vida Por todas las maravillas y bendiciones  que nos das a diario</t>
+          <t>Breaking News God is going to Double your Blessings this week, get ready to Receive them.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>I don't know who you are or what your name is but if you're Reading this, I send healing to your entire body in the name of Jesus</t>
+          <t>Casper Miguel</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Amén, amén,gloria al señor Jesucristo</t>
+          <t>Amén</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Casper Miguel</t>
+          <t>Amen amen gloria a Dios</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amén </t>
+          <t>INFINITAS GRACIAS SEÑOR JESÚS por un día más de vida Por todas las maravillas y bendiciones  que nos das a diario</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Thank you my eternal GOD because your favor reaches us, every day and your great mercy there is no way to repay what you do for us, why I recognize that day by d… See more</t>
+          <t>Move in us Holy Spirit, fill our soul with your beautiful presence.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Amén gloria a Dios aleluya gracias señor Jesús por todo.</t>
+          <t>Thank you my eternal GOD because your favor reaches us, every day and your great mercy there is no way to repay what you do for us, why I recognize that day by d… See more</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Casper Miguel</t>
+          <t xml:space="preserve">Amén amén aleluya yo sin ti no soy nada padre celestial ayudame señor de señores eres mi rey mi salvador te amo tanto que quiero estar junto a ti padre celestial amén </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">THE RAPTURE IS NEAR CHRIST COMES </t>
+          <t>You Are Not Alone@</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>You Are Not Alone@</t>
+          <t>Hello blessings good day I invite you to follow this page as it has been of great blessing to my life</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hello blessings good day I invite you to follow this page as it has been of great blessing to my life</t>
+          <t>Gracias gracias gracias por llegar bien a casa y librarme de todo mal amén gloria a Dios</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amén Padre Bendito </t>
+          <t>Amén, amén y amén</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Amen Amen Dios siempre  dándome  una oportunidad  más.  Levantarnos de la cama bendito Dios  de verdad  por ese gran amor que nos  tiene</t>
+          <t>Amén amado Dios gracias por tus misericordias.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Bendecido viernes..</t>
+          <t xml:space="preserve">Amén Padre Bendito </t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Good Morning Happy Friday </t>
+          <t>Amén amén gracias padre amado Dios</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amén Padre Bendito </t>
+          <t>Igualmente señor pongo todo a tus mano gloria a dios</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gloria a Dios Amén y Amén </t>
+          <t>Amen gracias love</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Amen</t>
+          <t xml:space="preserve">Amén Padre Bendito </t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amén y Amén </t>
+          <t xml:space="preserve">Good Morning Happy Friday </t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Igualmente señor pongo todo a tus mano gloria a dios</t>
+          <t>Amén  así es gracias padre celestial</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Que así sea mil bendiciones</t>
+          <t>Bendecido viernes..</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amén Padre Bendito </t>
+          <t>Bendiciones..</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Amen gracias love</t>
+          <t>Amén</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Amén amén gracias padre amado Dios</t>
+          <t>Amen amen amen</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Amén</t>
+          <t xml:space="preserve">Amén </t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amén </t>
+          <t>Amen  Amen  Amen</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Amén  así es gracias padre celestial</t>
+          <t>Gracias padre celestial amén</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Amén, amén y amén</t>
+          <t>Amén amén padres celestial x tdo tu bendición y también cuidados a mis hijos a cada uno de ellos</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Amen amen Amen</t>
+          <t xml:space="preserve">Amén Padre Bendito </t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Amen</t>
+          <t>Amén padre amado amén amén</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Amen amen amen</t>
+          <t>Amen Amen Dios siempre  dándome  una oportunidad  más.  Levantarnos de la cama bendito Dios  de verdad  por ese gran amor que nos  tiene</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>AMÉN,AMÉN,GLORIA Al PADRE CELESTIAL</t>
+          <t xml:space="preserve">Amén Padre Bendito </t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Amén amado Dios gracias por tus misericordias.</t>
+          <t>Amen amen Amen</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amén gloria a Dios igualmente para usted y tú familia excelente día Dios los bendiga hoy mañana y siempre gracias por compartir tanta belleza </t>
+          <t>Amén, Amén, Amén</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Amén padre amado amén amén</t>
+          <t>AMEN AMEN</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amén </t>
+          <t xml:space="preserve">Gloria a Dios Amén y Amén </t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amén y Amén </t>
+          <t>Amen gloria a Dios</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Bendiciones..</t>
+          <t>Amén Gloria al Padre Celestial x toda su misericordia y protección .</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Amen </t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>A men</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Amén..</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Happy day... </t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Amén, Amén, Amén</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
         <is>
           <t xml:space="preserve">Amen 
  si mi señor danos fuerzas Para todos ayudanos en estos momentos mas aorita k van aoperar ami mama k ya es mayor de edad Para k salga bien de su operacion telo pedimos señor en El nombre de nuetro seño jesu crito amen 
@@ -771,181 +736,185 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Amen amen</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amén y Amén </t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amén Padre Bendito </t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Amén amén amén</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Amén padre</t>
+        </is>
+      </c>
+    </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amén gloria a Dios </t>
+          <t>solo tu nos da un amor incondicional gracias padre  Celestial gracias por tu inmenso Amor Aleluya Gloria Dios</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blessed Friday... 
- </t>
+          <t>Amén gloria a Dios bendiciones</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gloria a Dios Amen </t>
+          <t>Amén amén amén</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Maravilloso Dios Amado  Amén...</t>
+          <t>Gracias gracias dios amén amén</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Gloria a Dios Amen padre Bendito</t>
+          <t>AMÉN AMÉN Y AMÉN GRACIAS GRACIAS Y GRACIAS……</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Aleluya amen</t>
+          <t>Amén aleluya gloria a Dios</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Amén padre</t>
+          <t>AMÉN AMÉN</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Amén amén</t>
+          <t xml:space="preserve">AMÉN  GRACIAS INFINITAS SEÑOR JESÚS  </t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Amén Gloria a Dios</t>
+          <t>amen Gloria adios amen</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Amén, amén</t>
+          <t>Gloria a Dios Amen padre Bendito</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Así es Señor. Amén Amén Gloria a Dios Aleluya.</t>
+          <t>Amén padre amado</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Amen</t>
+          <t>Amen amen</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Amén padre amado</t>
+          <t>Así es padre celestial amen</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Amén amén gloria a dios</t>
+          <t>Ame amen gloria a Dios</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Amén  Señor Dios todopoderoso</t>
+          <t>Amén amén aleluya aleluya gloria a Dios</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t xml:space="preserve">AMÉN 
- GRACIAS INFINITAS SEÑOR JESÚS 
- </t>
+          <t>Amén Amén</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>AMÉN AMÉN Y AMÉN GRACIAS GRACIAS Y GRACIAS……</t>
+          <t>Amén gloria ti señor Jesucristo Amén muchas gracias AMEN</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Believe and see the Glory of God</t>
+          <t>Dios es real</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Amén gloria ADios</t>
+          <t>Un Joven Cristiano.</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Amen</t>
+          <t>Amen gloria a dios padre celestial</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Dios es real</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Amen gloria a dios padre celestial</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
           <t>Un Joven Cristiano.</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Return to your first love</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Gustavo Melo</t>
         </is>
       </c>
     </row>

</xml_diff>